<commit_message>
test folder_minc 50d compare with single porosity and minc250d compare with 50ini_fiv_spot
</commit_message>
<xml_diff>
--- a/trials/minc/minc_5_spot/minc_5_spot_250d/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials/minc/minc_5_spot/minc_5_spot_250d/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/minc_5_spot_250d/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAB56631-CB7D-4ED3-8621-10D2130E3EF6}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73F35EDD-BEE6-45B1-BCCB-736D5B0A1B26}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="d" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="singleVs50d" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>xporT</t>
   </si>
@@ -119,6 +120,18 @@
   <si>
     <t>Pressure</t>
   </si>
+  <si>
+    <t>wai_single_P</t>
+  </si>
+  <si>
+    <t>wai_single_T</t>
+  </si>
+  <si>
+    <t>wai_50d_P</t>
+  </si>
+  <si>
+    <t>wai_50d_T</t>
+  </si>
 </sst>
 </file>
 
@@ -152,8 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +400,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$1</c:f>
+              <c:f>Sheet1!$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -421,7 +435,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$11</c:f>
+              <c:f>Sheet1!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -460,7 +474,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$11</c:f>
+              <c:f>Sheet1!$U$2:$U$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -644,7 +658,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$1</c:f>
+              <c:f>Sheet1!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -685,7 +699,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$11</c:f>
+              <c:f>Sheet1!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -724,7 +738,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$X$2:$X$11</c:f>
+              <c:f>Sheet1!$Y$2:$Y$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -944,7 +958,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$Q$1</c15:sqref>
+                          <c15:sqref>Sheet1!$R$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -983,7 +997,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$P$2:$P$13</c15:sqref>
+                          <c15:sqref>Sheet1!$Q$2:$Q$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1034,7 +1048,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$Q$2:$Q$13</c15:sqref>
+                          <c15:sqref>Sheet1!$R$2:$R$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1097,7 +1111,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$V$1</c15:sqref>
+                          <c15:sqref>Sheet1!$W$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1136,7 +1150,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$S$2:$S$11</c15:sqref>
+                          <c15:sqref>Sheet1!$T$2:$T$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1181,7 +1195,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$V$2:$V$11</c15:sqref>
+                          <c15:sqref>Sheet1!$W$2:$W$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1391,7 +1405,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$Z$1</c15:sqref>
+                          <c15:sqref>Sheet1!$AA$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1434,7 +1448,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$S$2:$S$11</c15:sqref>
+                          <c15:sqref>Sheet1!$T$2:$T$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1479,7 +1493,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$Z$2:$Z$11</c15:sqref>
+                          <c15:sqref>Sheet1!$AA$2:$AA$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1536,7 +1550,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$N$1</c15:sqref>
+                          <c15:sqref>Sheet1!$O$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1579,7 +1593,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$M$2:$M$13</c15:sqref>
+                          <c15:sqref>Sheet1!$N$2:$N$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1630,7 +1644,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$N$2:$N$13</c15:sqref>
+                          <c15:sqref>Sheet1!$O$2:$O$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2133,7 +2147,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$1</c:f>
+              <c:f>Sheet1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2168,7 +2182,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$13</c:f>
+              <c:f>Sheet1!$Q$2:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2213,7 +2227,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$13</c:f>
+              <c:f>Sheet1!$R$2:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2268,7 +2282,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$1</c:f>
+              <c:f>Sheet1!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2303,7 +2317,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$11</c:f>
+              <c:f>Sheet1!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2342,7 +2356,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$2:$V$11</c:f>
+              <c:f>Sheet1!$W$2:$W$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2526,7 +2540,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Z$1</c:f>
+              <c:f>Sheet1!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2567,7 +2581,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$11</c:f>
+              <c:f>Sheet1!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2606,7 +2620,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$11</c:f>
+              <c:f>Sheet1!$AA$2:$AA$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2655,7 +2669,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>Sheet1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2696,7 +2710,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:f>Sheet1!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2741,7 +2755,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$13</c:f>
+              <c:f>Sheet1!$O$2:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2981,7 +2995,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$T$1</c15:sqref>
+                          <c15:sqref>Sheet1!$U$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3022,7 +3036,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$S$2:$S$11</c15:sqref>
+                          <c15:sqref>Sheet1!$T$2:$T$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3067,7 +3081,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$T$2:$T$11</c15:sqref>
+                          <c15:sqref>Sheet1!$U$2:$U$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3279,7 +3293,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$X$1</c15:sqref>
+                          <c15:sqref>Sheet1!$Y$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3326,7 +3340,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$S$2:$S$11</c15:sqref>
+                          <c15:sqref>Sheet1!$T$2:$T$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3371,7 +3385,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$X$2:$X$11</c15:sqref>
+                          <c15:sqref>Sheet1!$Y$2:$Y$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4122,7 +4136,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:f>Sheet1!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4167,7 +4181,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$14</c:f>
+              <c:f>Sheet1!$O$2:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4620,7 +4634,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:f>Sheet1!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4665,7 +4679,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$14</c:f>
+              <c:f>Sheet1!$O$2:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5676,7 +5690,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:f>Sheet1!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5721,7 +5735,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$13</c:f>
+              <c:f>Sheet1!$O$2:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -6075,6 +6089,1486 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>singleVs50d!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wai_single_T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>singleVs50d!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>671.75144212722205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>601.04076400856604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.33008588990299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>459.61940777123499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>388.90872965254999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.19805153384402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247.48737341514601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.77669529649299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.06601717790799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.355339059315398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>singleVs50d!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>117.645219416213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126.915503255047</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181.76451989085101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>254.49624496736101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>289.62462100477802</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>298.30833308566099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>297.58129596884299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>294.95871276486702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>289.64558827614002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>272.50703290104798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DC1-4803-9B7E-09C466551E32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>singleVs50d!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wai_50d_T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>singleVs50d!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>671.75144212722205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>601.04076400856604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.33008588990299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>459.61940777123499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>388.90872965254999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.19805153384402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247.48737341514601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.77669529649299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.06601717790799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.355339059315398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>singleVs50d!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>118.787001679734</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130.792854445107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.83650735595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208.43571950973501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>245.482128133674</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>268.40311104290799</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>280.86131431869302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>286.15587861806301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>278.93278992566599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250.98468484445601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9DC1-4803-9B7E-09C466551E32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>porousT_literature</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248.87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>386.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>526.88</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>606.39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>658.17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>686.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>264.97000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>280.66000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>290.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>294.08999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>293.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>285.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>266.54000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>225.57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>167.42</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>126.14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>115.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9DC1-4803-9B7E-09C466551E32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T50_literature</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176.47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.88</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>385.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>458.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>527.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>606.46</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>656.23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>686.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>268.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>283.27999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>290.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>294.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>290.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>281.83999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>261.58999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>221.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>167.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>127.89</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>116.71</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9DC1-4803-9B7E-09C466551E32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1529284239"/>
+        <c:axId val="1529282991"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1529284239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="700"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1529282991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1529282991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="300"/>
+          <c:min val="110"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1529284239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>singleVs50d!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wai_single_P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>singleVs50d!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>671.75144212722205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>601.04076400856604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.33008588990299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>459.61940777123499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>388.90872965254999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.19805153384402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247.48737341514601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.77669529649299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.06601717790799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.355339059315398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>singleVs50d!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.7540902045159097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0423268650203603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7496180061046491</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6095341869923097</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5204448127480905</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4397354599474301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3037693398124208</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9989579732367702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.4077065191315503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7250496808952596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D929-4EF9-9169-8F4C8ADCA76F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>singleVs50d!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wai_50d_P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>singleVs50d!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>671.75144212722205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>601.04076400856604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.33008588990299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>459.61940777123499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>388.90872965254999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.19805153384402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247.48737341514601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.77669529649299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.06601717790799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.355339059315398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>singleVs50d!$J$2:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.7870668997680603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0851879349178493</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7930648628841199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6277377628885503</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5079901603093102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3914397603401296</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.2458638011425203</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0379394183405504</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3174362424825503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0441945657076896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D929-4EF9-9169-8F4C8ADCA76F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>porousP_literature</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>249.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>319.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>385.27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>529.67999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>607.54999999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>659.56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.66</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D929-4EF9-9169-8F4C8ADCA76F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P50_literature</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>17.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>102.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>249.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>319.22000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>386.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>527.67999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>606.49</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>658.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.4600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.43</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D929-4EF9-9169-8F4C8ADCA76F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2074396767"/>
+        <c:axId val="2074390111"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2074396767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="700"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2074390111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2074390111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2074396767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6275,6 +7769,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8340,6 +9914,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8865,7 +11471,7 @@
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -8895,13 +11501,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>423864</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
@@ -9044,6 +11650,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90586638-235C-4C48-86FF-2F4CBDD79D08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131045FF-AE3D-4982-AB40-1046BC578D2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9349,21 +12032,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5CB30-10C3-41ED-9059-520434D88C4C}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="M43" sqref="M43:M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9388,41 +12072,41 @@
       <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>19.89</v>
       </c>
@@ -9447,43 +12131,43 @@
       <c r="K2">
         <v>5.2</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>18.190000000000001</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>6.14</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>17.23</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>5.53</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>671.65</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>117.62316994</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>9827464.2497252505</v>
       </c>
-      <c r="V2">
-        <f>U2*0.000001</f>
+      <c r="W2">
+        <f>V2*0.000001</f>
         <v>9.8274642497252493</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>120.80381057</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>8939604.2250047792</v>
       </c>
-      <c r="Z2">
-        <f>Y2*0.000001</f>
+      <c r="AA2">
+        <f>Z2*0.000001</f>
         <v>8.9396042250047785</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>47.53</v>
       </c>
@@ -9508,43 +12192,43 @@
       <c r="K3">
         <v>6.64</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>46.76</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>6.48</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>47.3</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>6.83</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>600.95000000000005</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>124.4572096</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>9115232.39208184</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V11" si="0">U3*0.000001</f>
+      <c r="W3">
+        <f t="shared" ref="W3:W11" si="0">V3*0.000001</f>
         <v>9.1152323920818397</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>134.95708734999999</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>8252656.5485431002</v>
       </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3:Z11" si="1">Y3*0.000001</f>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA11" si="1">Z3*0.000001</f>
         <v>8.2526565485431007</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103.9</v>
       </c>
@@ -9569,43 +12253,43 @@
       <c r="K4">
         <v>7.55</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>103.24</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>6.75</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>102.73</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>7.67</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>530.25</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>162.87853483000001</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>8811837.4275563192</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <f t="shared" si="0"/>
         <v>8.811837427556318</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>158.19392737000001</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>7969374.5377587499</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <f t="shared" si="1"/>
         <v>7.9693745377587497</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>176.46</v>
       </c>
@@ -9630,43 +12314,43 @@
       <c r="K5">
         <v>8.0399999999999991</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>174.1</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>6.93</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>174.84</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>8.0299999999999994</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>459.55</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>224.45695542999999</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>8652505.8198963497</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <f t="shared" si="0"/>
         <v>8.6525058198963496</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>187.12071614999999</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>7804063.5463587297</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <f t="shared" si="1"/>
         <v>7.8040635463587291</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>248.87</v>
       </c>
@@ -9691,43 +12375,43 @@
       <c r="K6">
         <v>8.19</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>247.77</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>7.05</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>249.52</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>8.18</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>388.85</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>269.09023970999999</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>8548554.6140046101</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <f t="shared" si="0"/>
         <v>8.54855461400461</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>216.11043715</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>7689311.0660804603</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <f t="shared" si="1"/>
         <v>7.6893110660804602</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>320</v>
       </c>
@@ -9752,43 +12436,43 @@
       <c r="K7">
         <v>8.3000000000000007</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>317.48</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>7.11</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>319.22000000000003</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>8.24</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>318.14999999999998</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>289.22545461999999</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>8455698.9586727601</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <f t="shared" si="0"/>
         <v>8.4556989586727589</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>240.18284641</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>7593878.8461502995</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <f t="shared" si="1"/>
         <v>7.5938788461502993</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>386.85</v>
       </c>
@@ -9813,43 +12497,43 @@
       <c r="K8">
         <v>8.43</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>384.4</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>7.25</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>386.12</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>8.36</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>247.45</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>296.25291792000002</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>8348090.7328550396</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <f t="shared" si="0"/>
         <v>8.3480907328550398</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>257.55136529999999</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>7497947.4602348097</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <f t="shared" si="1"/>
         <v>7.4979474602348093</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>459.61</v>
       </c>
@@ -9874,43 +12558,43 @@
       <c r="K9">
         <v>8.5</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>459.02</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>7.36</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>459.76</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>8.4600000000000009</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>176.75</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>296.70751174999998</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>8201243.3307479396</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <f t="shared" si="0"/>
         <v>8.2012433307479391</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>269.44583455999998</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>7382684.6680199401</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <f t="shared" si="1"/>
         <v>7.3826846680199401</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>526.88</v>
       </c>
@@ -9935,43 +12619,43 @@
       <c r="K10">
         <v>8.66</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>526.97</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>7.53</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>527.67999999999995</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>8.6199999999999992</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>106.05</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>292.78597030999998</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>7752974.76154783</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <f t="shared" si="0"/>
         <v>7.7529747615478293</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>278.19900498999999</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>7214369.6961599803</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <f t="shared" si="1"/>
         <v>7.2143696961599799</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>606.39</v>
       </c>
@@ -9996,43 +12680,43 @@
       <c r="K11">
         <v>9</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>604.77</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>7.83</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>606.49</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>8.94</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>35.35</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>280.41975886</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>6460937.0620371802</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <f t="shared" si="0"/>
         <v>6.4609370620371802</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>284.00292216999998</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>6850044.5600787597</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <f t="shared" si="1"/>
         <v>6.8500445600787589</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>658.17</v>
       </c>
@@ -10057,20 +12741,20 @@
       <c r="K12">
         <v>9.5</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>658.66</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>8.2899999999999991</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>658.5</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>9.43</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>686.13</v>
       </c>
@@ -10095,32 +12779,392 @@
       <c r="K13">
         <v>9.92</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>687.55</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>8.84</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>687.11</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U16">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="V16">
         <v>7969374.5377587499</v>
       </c>
     </row>
-    <row r="17" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U17">
+    <row r="17" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V17">
         <v>7593878.8461502995</v>
       </c>
     </row>
-    <row r="18" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U18">
+    <row r="18" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V18">
         <v>7214369.6961599803</v>
+      </c>
+    </row>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>19.89</v>
+      </c>
+      <c r="G43">
+        <f>F43</f>
+        <v>19.89</v>
+      </c>
+      <c r="H43">
+        <v>264.97000000000003</v>
+      </c>
+      <c r="I43">
+        <f>H43</f>
+        <v>264.97000000000003</v>
+      </c>
+      <c r="K43">
+        <v>19.64</v>
+      </c>
+      <c r="L43">
+        <f>K43</f>
+        <v>19.64</v>
+      </c>
+      <c r="M43">
+        <v>5.2</v>
+      </c>
+      <c r="N43">
+        <f>M43</f>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>47.53</v>
+      </c>
+      <c r="G44" t="str">
+        <f>G43&amp;", "&amp;F44</f>
+        <v>19.89, 47.53</v>
+      </c>
+      <c r="H44">
+        <v>280.66000000000003</v>
+      </c>
+      <c r="I44" t="str">
+        <f>I43&amp;", "&amp;H44</f>
+        <v>264.97, 280.66</v>
+      </c>
+      <c r="K44">
+        <v>47.97</v>
+      </c>
+      <c r="L44" t="str">
+        <f>L43&amp;", "&amp;K44</f>
+        <v>19.64, 47.97</v>
+      </c>
+      <c r="M44">
+        <v>6.64</v>
+      </c>
+      <c r="N44" t="str">
+        <f>N43&amp;", "&amp;M44</f>
+        <v>5.2, 6.64</v>
+      </c>
+    </row>
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>103.9</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" ref="G45:G54" si="2">G44&amp;", "&amp;F45</f>
+        <v>19.89, 47.53, 103.9</v>
+      </c>
+      <c r="H45">
+        <v>290.16000000000003</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" ref="I45:I54" si="3">I44&amp;", "&amp;H45</f>
+        <v>264.97, 280.66, 290.16</v>
+      </c>
+      <c r="K45">
+        <v>104.48</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" ref="L45:L54" si="4">L44&amp;", "&amp;K45</f>
+        <v>19.64, 47.97, 104.48</v>
+      </c>
+      <c r="M45">
+        <v>7.55</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" ref="N45:N54" si="5">N44&amp;", "&amp;M45</f>
+        <v>5.2, 6.64, 7.55</v>
+      </c>
+    </row>
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>176.46</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46</v>
+      </c>
+      <c r="H46">
+        <v>294.08999999999997</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09</v>
+      </c>
+      <c r="K46">
+        <v>174.85</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85</v>
+      </c>
+      <c r="M46">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04</v>
+      </c>
+    </row>
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>248.87</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87</v>
+      </c>
+      <c r="H47">
+        <v>293.94</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94</v>
+      </c>
+      <c r="K47">
+        <v>249.53</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53</v>
+      </c>
+      <c r="M47">
+        <v>8.19</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19</v>
+      </c>
+    </row>
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>320</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320</v>
+      </c>
+      <c r="H48">
+        <v>285.63</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63</v>
+      </c>
+      <c r="K48">
+        <v>319.31</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31</v>
+      </c>
+      <c r="M48">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3</v>
+      </c>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>386.85</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320, 386.85</v>
+      </c>
+      <c r="H49">
+        <v>266.54000000000002</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63, 266.54</v>
+      </c>
+      <c r="K49">
+        <v>385.27</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31, 385.27</v>
+      </c>
+      <c r="M49">
+        <v>8.43</v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3, 8.43</v>
+      </c>
+    </row>
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>459.61</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320, 386.85, 459.61</v>
+      </c>
+      <c r="H50">
+        <v>225.57</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63, 266.54, 225.57</v>
+      </c>
+      <c r="K50">
+        <v>459.82</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31, 385.27, 459.82</v>
+      </c>
+      <c r="M50">
+        <v>8.5</v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3, 8.43, 8.5</v>
+      </c>
+    </row>
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>526.88</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320, 386.85, 459.61, 526.88</v>
+      </c>
+      <c r="H51">
+        <v>167.42</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63, 266.54, 225.57, 167.42</v>
+      </c>
+      <c r="K51">
+        <v>529.67999999999995</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31, 385.27, 459.82, 529.68</v>
+      </c>
+      <c r="M51">
+        <v>8.66</v>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3, 8.43, 8.5, 8.66</v>
+      </c>
+    </row>
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>606.39</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320, 386.85, 459.61, 526.88, 606.39</v>
+      </c>
+      <c r="H52">
+        <v>126.14</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63, 266.54, 225.57, 167.42, 126.14</v>
+      </c>
+      <c r="K52">
+        <v>607.54999999999995</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31, 385.27, 459.82, 529.68, 607.55</v>
+      </c>
+      <c r="M52">
+        <v>9</v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3, 8.43, 8.5, 8.66, 9</v>
+      </c>
+    </row>
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>658.17</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320, 386.85, 459.61, 526.88, 606.39, 658.17</v>
+      </c>
+      <c r="H53">
+        <v>117</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63, 266.54, 225.57, 167.42, 126.14, 117</v>
+      </c>
+      <c r="K53">
+        <v>659.56</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31, 385.27, 459.82, 529.68, 607.55, 659.56</v>
+      </c>
+      <c r="M53">
+        <v>9.5</v>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3, 8.43, 8.5, 8.66, 9, 9.5</v>
+      </c>
+    </row>
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>686.13</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="2"/>
+        <v>19.89, 47.53, 103.9, 176.46, 248.87, 320, 386.85, 459.61, 526.88, 606.39, 658.17, 686.13</v>
+      </c>
+      <c r="H54">
+        <v>115.77</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="3"/>
+        <v>264.97, 280.66, 290.16, 294.09, 293.94, 285.63, 266.54, 225.57, 167.42, 126.14, 117, 115.77</v>
+      </c>
+      <c r="K54">
+        <v>687.3</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="4"/>
+        <v>19.64, 47.97, 104.48, 174.85, 249.53, 319.31, 385.27, 459.82, 529.68, 607.55, 659.56, 687.3</v>
+      </c>
+      <c r="M54">
+        <v>9.92</v>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="5"/>
+        <v>5.2, 6.64, 7.55, 8.04, 8.19, 8.3, 8.43, 8.5, 8.66, 9, 9.5, 9.92</v>
       </c>
     </row>
   </sheetData>
@@ -10133,8 +13177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7871E86D-6023-4C89-A9C8-AAC74AB9E535}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10752,7 +13796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8403754-388F-45EC-8E75-F6F3E2570208}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -11576,10 +14620,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC65E012-91EC-4E31-BE29-88D2C65508E0}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="A28:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12427,6 +15471,116 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:G23">
     <sortCondition descending="1" ref="G2:G23"/>
@@ -12435,4 +15589,234 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF288C2-0066-47C7-BF38-8B661EC23845}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>671.75144212722205</v>
+      </c>
+      <c r="B2">
+        <v>9.7540902045159097</v>
+      </c>
+      <c r="C2">
+        <v>117.645219416213</v>
+      </c>
+      <c r="I2">
+        <v>671.75144212722205</v>
+      </c>
+      <c r="J2">
+        <v>8.7870668997680603</v>
+      </c>
+      <c r="K2">
+        <v>118.787001679734</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>601.04076400856604</v>
+      </c>
+      <c r="B3">
+        <v>9.0423268650203603</v>
+      </c>
+      <c r="C3">
+        <v>126.915503255047</v>
+      </c>
+      <c r="I3">
+        <v>601.04076400856604</v>
+      </c>
+      <c r="J3">
+        <v>8.0851879349178493</v>
+      </c>
+      <c r="K3">
+        <v>130.792854445107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>530.33008588990299</v>
+      </c>
+      <c r="B4">
+        <v>8.7496180061046491</v>
+      </c>
+      <c r="C4">
+        <v>181.76451989085101</v>
+      </c>
+      <c r="I4">
+        <v>530.33008588990299</v>
+      </c>
+      <c r="J4">
+        <v>7.7930648628841199</v>
+      </c>
+      <c r="K4">
+        <v>163.83650735595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>459.61940777123499</v>
+      </c>
+      <c r="B5">
+        <v>8.6095341869923097</v>
+      </c>
+      <c r="C5">
+        <v>254.49624496736101</v>
+      </c>
+      <c r="I5">
+        <v>459.61940777123499</v>
+      </c>
+      <c r="J5">
+        <v>7.6277377628885503</v>
+      </c>
+      <c r="K5">
+        <v>208.43571950973501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>388.90872965254999</v>
+      </c>
+      <c r="B6">
+        <v>8.5204448127480905</v>
+      </c>
+      <c r="C6">
+        <v>289.62462100477802</v>
+      </c>
+      <c r="I6">
+        <v>388.90872965254999</v>
+      </c>
+      <c r="J6">
+        <v>7.5079901603093102</v>
+      </c>
+      <c r="K6">
+        <v>245.482128133674</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>318.19805153384402</v>
+      </c>
+      <c r="B7">
+        <v>8.4397354599474301</v>
+      </c>
+      <c r="C7">
+        <v>298.30833308566099</v>
+      </c>
+      <c r="I7">
+        <v>318.19805153384402</v>
+      </c>
+      <c r="J7">
+        <v>7.3914397603401296</v>
+      </c>
+      <c r="K7">
+        <v>268.40311104290799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>247.48737341514601</v>
+      </c>
+      <c r="B8">
+        <v>8.3037693398124208</v>
+      </c>
+      <c r="C8">
+        <v>297.58129596884299</v>
+      </c>
+      <c r="I8">
+        <v>247.48737341514601</v>
+      </c>
+      <c r="J8">
+        <v>7.2458638011425203</v>
+      </c>
+      <c r="K8">
+        <v>280.86131431869302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>176.77669529649299</v>
+      </c>
+      <c r="B9">
+        <v>7.9989579732367702</v>
+      </c>
+      <c r="C9">
+        <v>294.95871276486702</v>
+      </c>
+      <c r="I9">
+        <v>176.77669529649299</v>
+      </c>
+      <c r="J9">
+        <v>7.0379394183405504</v>
+      </c>
+      <c r="K9">
+        <v>286.15587861806301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>106.06601717790799</v>
+      </c>
+      <c r="B10">
+        <v>7.4077065191315503</v>
+      </c>
+      <c r="C10">
+        <v>289.64558827614002</v>
+      </c>
+      <c r="I10">
+        <v>106.06601717790799</v>
+      </c>
+      <c r="J10">
+        <v>6.3174362424825503</v>
+      </c>
+      <c r="K10">
+        <v>278.93278992566599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35.355339059315398</v>
+      </c>
+      <c r="B11">
+        <v>5.7250496808952596</v>
+      </c>
+      <c r="C11">
+        <v>272.50703290104798</v>
+      </c>
+      <c r="I11">
+        <v>35.355339059315398</v>
+      </c>
+      <c r="J11">
+        <v>4.0441945657076896</v>
+      </c>
+      <c r="K11">
+        <v>250.98468484445601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>